<commit_message>
added the field profesori in the disciplina table as ManyToManyField
</commit_message>
<xml_diff>
--- a/media/Web programming/Web programming.xlsx
+++ b/media/Web programming/Web programming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40729\Desktop\Licenta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEF69C2-549E-4A7C-9969-1D8A81C5D12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69F7513-2092-4FE3-A483-4B8859A8D0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,12 +469,12 @@
   <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>